<commit_message>
MLM with Mutiple Models
</commit_message>
<xml_diff>
--- a/GenAI.xlsx
+++ b/GenAI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91956\OneDrive\DATA-SCIENCE-NARESHIT-OMKAR\GITHUB\GenAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C997AE-D2D1-45F8-ACB2-8C137346E264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD714D27-7792-407A-BA1E-AB365AF1B7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>S.NO</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>Document search with embeddings - Base using Jupyter Notebook</t>
+  </si>
+  <si>
+    <t>Chroma + LangChain + RAG + Text</t>
+  </si>
+  <si>
+    <t>Chroma + LangChain + RAG + PDF</t>
   </si>
 </sst>
 </file>
@@ -459,7 +465,7 @@
   <dimension ref="B1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -600,17 +606,29 @@
       <c r="B10" s="4">
         <v>9</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="C10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="2:5" ht="21" x14ac:dyDescent="0.4">
       <c r="B11" s="4">
         <v>10</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="2:5" ht="21" x14ac:dyDescent="0.4">
       <c r="B12" s="4">

</xml_diff>

<commit_message>
YoloV3 - Object-Detection using streamlit
</commit_message>
<xml_diff>
--- a/GenAI.xlsx
+++ b/GenAI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91956\OneDrive\DATA-SCIENCE-NARESHIT-OMKAR\GITHUB\GenAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD714D27-7792-407A-BA1E-AB365AF1B7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C0A892-0B0B-42EB-AEC1-55D3524F8624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>S.NO</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Chroma + LangChain + RAG + PDF</t>
+  </si>
+  <si>
+    <t>Masked Language Modeling using BERT mutiple model</t>
   </si>
 </sst>
 </file>
@@ -465,7 +468,7 @@
   <dimension ref="B1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,9 +637,15 @@
       <c r="B12" s="4">
         <v>11</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" spans="2:5" ht="21" x14ac:dyDescent="0.4">
       <c r="B13" s="4">

</xml_diff>